<commit_message>
more work on methods
</commit_message>
<xml_diff>
--- a/Worm strains.xlsx
+++ b/Worm strains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blandt/Desktop/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75AC662-5171-0F44-B9FE-C729FD010227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402FEEBA-008D-2A42-A356-1F25C0B0CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" firstSheet="4" activeTab="12" xr2:uid="{60ADC3BD-DE4A-FA4C-8EE3-6C93FC3E3F3B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" firstSheet="4" activeTab="9" xr2:uid="{60ADC3BD-DE4A-FA4C-8EE3-6C93FC3E3F3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mutant lines" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,17 @@
     <sheet name="PAR-2 guides" sheetId="3" r:id="rId4"/>
     <sheet name="PAR-2 repair templates" sheetId="4" r:id="rId5"/>
     <sheet name="PAR-2 screening primers" sheetId="5" r:id="rId6"/>
-    <sheet name="glh method guides" sheetId="7" r:id="rId7"/>
-    <sheet name="glh method repair templates" sheetId="8" r:id="rId8"/>
-    <sheet name="Insect cell lysis buffer" sheetId="9" r:id="rId9"/>
-    <sheet name="Insect cell elution buffer" sheetId="10" r:id="rId10"/>
-    <sheet name="Ubiquitin assay" sheetId="11" r:id="rId11"/>
-    <sheet name="E coli lysis buffer" sheetId="12" r:id="rId12"/>
-    <sheet name="E coli elution buffer" sheetId="13" r:id="rId13"/>
+    <sheet name="Y65A" sheetId="14" r:id="rId7"/>
+    <sheet name="glh method guides" sheetId="7" r:id="rId8"/>
+    <sheet name="glh method repair templates" sheetId="8" r:id="rId9"/>
+    <sheet name="GCN4" sheetId="15" r:id="rId10"/>
+    <sheet name="Insect cell lysis buffer" sheetId="9" r:id="rId11"/>
+    <sheet name="Insect cell elution buffer" sheetId="10" r:id="rId12"/>
+    <sheet name="Ubiquitin assay" sheetId="11" r:id="rId13"/>
+    <sheet name="E coli lysis buffer" sheetId="12" r:id="rId14"/>
+    <sheet name="E coli elution buffer" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="304">
   <si>
     <t>Strain</t>
   </si>
@@ -923,13 +924,49 @@
   </si>
   <si>
     <t>1 tablet per 50 ml buffer</t>
+  </si>
+  <si>
+    <t>TB0033</t>
+  </si>
+  <si>
+    <t>CGTCGAGGGAGGACCACTCCCATTCGCCTTCGACATCCTCGCGACCTCTTTCATGGCTGGATCTAAGACCTTCATCAACCACACCCAAGGAATCCCAGACTTCTTCAAGC</t>
+  </si>
+  <si>
+    <t>TB0034</t>
+  </si>
+  <si>
+    <t>GGTCTTGGATCCGTACATGA</t>
+  </si>
+  <si>
+    <t>TB0035</t>
+  </si>
+  <si>
+    <t>GGTGTGGTTGATGAAGGTCT</t>
+  </si>
+  <si>
+    <t>TB0135</t>
+  </si>
+  <si>
+    <t>TB0134</t>
+  </si>
+  <si>
+    <t>TB0138</t>
+  </si>
+  <si>
+    <t>AGCTGCTCTCGATATTCTCC</t>
+  </si>
+  <si>
+    <t>GGTCCGAAAATTGAAAAACC</t>
+  </si>
+  <si>
+    <t>TTTTCGTTTCAGATGGTCCGAAAATTGAAAAACCAAGAGGGATCCGGAGGACGTATGAAACAGCTTGAGGACAAGATTGAGGAATTACTCTCCAAGATTTATCACCTCGAGAACGAGATTGCCCGTCTCAAAAAATTAATCGGTGAGCGTGGTGGATCCGGTAATATCGAGAGCAGCTACGACGATTTGTTCATTTGTGA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -970,6 +1007,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -991,7 +1039,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1010,6 +1058,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1949,6 +1999,160 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FBB082-3224-864D-B538-52C9FFB100CE}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C1E3CA-FFC3-5345-81E5-79881393ED4A}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>280</v>
+      </c>
+      <c r="B11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16BFE7-56CD-2642-84BD-98F90F106235}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2015,7 +2219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AB85EA-4509-7645-B14C-1B5F418A76E1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -2106,7 +2310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB4D226-A41A-4746-964A-27FA90FB880A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2165,11 +2369,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDAC1FAA-FF26-2641-94A1-0E508AF13411}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
@@ -2665,6 +2869,45 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B571EE-378E-9B4D-90C8-6E8E8FF98535}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EEBBD22-5CE4-404B-9F55-038B3C3DCF57}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2731,7 +2974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D918171E-E9C0-2446-8229-90ED0F7AECB4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -2828,119 +3071,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C1E3CA-FFC3-5345-81E5-79881393ED4A}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="A1:B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>275</v>
-      </c>
-      <c r="B5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>276</v>
-      </c>
-      <c r="B6" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>283</v>
-      </c>
-      <c r="B7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>277</v>
-      </c>
-      <c r="B8" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>278</v>
-      </c>
-      <c r="B9" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>279</v>
-      </c>
-      <c r="B10" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>280</v>
-      </c>
-      <c r="B11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>281</v>
-      </c>
-      <c r="B12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>